<commit_message>
generate excel report 95%
</commit_message>
<xml_diff>
--- a/document/template.xlsx
+++ b/document/template.xlsx
@@ -223,13 +223,13 @@
     <numFmt numFmtId="184" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="185" formatCode="_([$Rp-421]* #,##0_);_([$Rp-421]* \(#,##0\);_([$Rp-421]* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="186" formatCode="_([$Rp-421]* #,##0.00_);_([$Rp-421]* \(#,##0.00\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="188" formatCode="0E+00"/>
-    <numFmt numFmtId="189" formatCode="0&quot;  &quot;"/>
-    <numFmt numFmtId="190" formatCode="0.0&quot;  &quot;"/>
-    <numFmt numFmtId="191" formatCode="0.00&quot;  &quot;"/>
-    <numFmt numFmtId="192" formatCode="0.000&quot;  &quot;"/>
-    <numFmt numFmtId="193" formatCode="_(&quot;Rp&quot;* #,##0.00_);_(&quot;Rp&quot;* \(#,##0.00\);_(&quot;Rp&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="194" formatCode="&quot;REAL.&quot;\ mmm\'\ yy"/>
+    <numFmt numFmtId="187" formatCode="0E+00"/>
+    <numFmt numFmtId="188" formatCode="0&quot;  &quot;"/>
+    <numFmt numFmtId="189" formatCode="0.0&quot;  &quot;"/>
+    <numFmt numFmtId="190" formatCode="0.00&quot;  &quot;"/>
+    <numFmt numFmtId="191" formatCode="0.000&quot;  &quot;"/>
+    <numFmt numFmtId="192" formatCode="_(&quot;Rp&quot;* #,##0.00_);_(&quot;Rp&quot;* \(#,##0.00\);_(&quot;Rp&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="193" formatCode="&quot;REAL.&quot;\ mmm\'\ yy"/>
   </numFmts>
   <fonts count="52">
     <font>
@@ -944,17 +944,17 @@
     <xf numFmtId="186" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="188" fontId="38" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="38" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="188" fontId="38" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="38" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="188" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="189" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="190" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="191" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="192" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="14" applyNumberFormat="0" applyBorder="0">
@@ -967,10 +967,10 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="188" fontId="38" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="38" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="188" fontId="38" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="38" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="37" fontId="43" fillId="0" borderId="0"/>
@@ -980,10 +980,10 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="193" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="194" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="194" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="194" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="192" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="193" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="193" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="193" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="186" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="186" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="186" fontId="3" fillId="0" borderId="0"/>
@@ -1000,7 +1000,7 @@
     <xf numFmtId="186" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="186" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1047,9 +1047,6 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="186" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1091,12 +1088,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="186" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1146,9 +1137,6 @@
     <xf numFmtId="41" fontId="34" fillId="0" borderId="0" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1200,54 +1188,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="33" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1259,15 +1205,6 @@
     </xf>
     <xf numFmtId="165" fontId="33" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1278,6 +1215,63 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="184">
@@ -2063,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2072,8 +2066,8 @@
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" customWidth="1"/>
     <col min="7" max="9" width="19.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
@@ -2098,11 +2092,11 @@
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="2:18" s="1" customFormat="1">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="78" t="s">
+      <c r="C4" s="86"/>
+      <c r="D4" s="74" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="14"/>
@@ -2110,11 +2104,11 @@
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="2:18" s="1" customFormat="1">
-      <c r="B5" s="99"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="85"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="94"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
@@ -2123,10 +2117,10 @@
       <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="88"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="97"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
@@ -2135,10 +2129,10 @@
       <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="95"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="88"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="97"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
@@ -2147,10 +2141,10 @@
       <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="88"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="97"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
@@ -2159,11 +2153,11 @@
       <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="98"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="105" t="s">
+      <c r="C9" s="80"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="84" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="15"/>
@@ -2173,368 +2167,371 @@
       <c r="B10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="104" t="s">
+      <c r="C10" s="79"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="99"/>
+      <c r="F10" s="99"/>
+      <c r="G10" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="104" t="s">
+      <c r="H10" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="104" t="s">
+      <c r="I10" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="104" t="s">
+      <c r="J10" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="104" t="s">
+      <c r="K10" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="104" t="s">
+      <c r="L10" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="M10" s="104" t="s">
+      <c r="M10" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="N10" s="104" t="s">
+      <c r="N10" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="O10" s="104" t="s">
+      <c r="O10" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="P10" s="104" t="s">
+      <c r="P10" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="Q10" s="104" t="s">
+      <c r="Q10" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="R10" s="104" t="s">
+      <c r="R10" s="83" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:18" s="20" customFormat="1">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="44"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="44"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="102"/>
+      <c r="O11" s="102"/>
+      <c r="P11" s="102"/>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="102"/>
     </row>
     <row r="12" spans="2:18" s="20" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B12" s="30"/>
-      <c r="C12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
-      <c r="R12" s="44"/>
+      <c r="F12" s="103"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="102"/>
+      <c r="K12" s="102"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="102"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="102"/>
+      <c r="P12" s="102"/>
+      <c r="Q12" s="102"/>
+      <c r="R12" s="102"/>
     </row>
     <row r="13" spans="2:18" s="20" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B13" s="30"/>
-      <c r="C13" s="29"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="44"/>
-    </row>
-    <row r="14" spans="2:18" s="49" customFormat="1">
-      <c r="B14" s="30"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="101" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="28"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="102"/>
+      <c r="P13" s="102"/>
+      <c r="Q13" s="102"/>
+      <c r="R13" s="102"/>
+    </row>
+    <row r="14" spans="2:18" s="46" customFormat="1">
+      <c r="B14" s="29"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="44"/>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="44"/>
-    </row>
-    <row r="15" spans="2:18" s="49" customFormat="1">
-      <c r="B15" s="30"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="101" t="s">
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="102"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="102"/>
+      <c r="P14" s="102"/>
+      <c r="Q14" s="102"/>
+      <c r="R14" s="102"/>
+    </row>
+    <row r="15" spans="2:18" s="46" customFormat="1">
+      <c r="B15" s="29"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="101"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
-    </row>
-    <row r="16" spans="2:18" s="49" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B16" s="30"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="47" t="s">
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="41"/>
+    </row>
+    <row r="16" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B16" s="29"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="48"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="44"/>
-      <c r="R16" s="44"/>
-    </row>
-    <row r="17" spans="2:18" s="49" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B17" s="30"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="51" t="s">
+      <c r="F16" s="45"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="41"/>
+    </row>
+    <row r="17" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B17" s="29"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="52"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
-      <c r="N17" s="44"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44"/>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="44"/>
-    </row>
-    <row r="18" spans="2:18" s="49" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B18" s="30"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="51" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+    </row>
+    <row r="18" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B18" s="29"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="52"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="44"/>
-      <c r="O18" s="44"/>
-      <c r="P18" s="44"/>
-      <c r="Q18" s="44"/>
-      <c r="R18" s="44"/>
-    </row>
-    <row r="19" spans="2:18" s="49" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B19" s="30"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="51" t="s">
+      <c r="F18" s="49"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+    </row>
+    <row r="19" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B19" s="29"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="52"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="44"/>
-      <c r="R19" s="44"/>
-    </row>
-    <row r="20" spans="2:18" s="49" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B20" s="30"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="51" t="s">
+      <c r="F19" s="49"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="41"/>
+    </row>
+    <row r="20" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B20" s="29"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="52"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="44"/>
-      <c r="O20" s="44"/>
-      <c r="P20" s="44"/>
-      <c r="Q20" s="44"/>
-      <c r="R20" s="44"/>
-    </row>
-    <row r="21" spans="2:18" s="49" customFormat="1">
-      <c r="B21" s="30"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="51" t="s">
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
+    </row>
+    <row r="21" spans="2:18" s="46" customFormat="1">
+      <c r="B21" s="29"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="52"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="44"/>
-      <c r="Q21" s="44"/>
-      <c r="R21" s="44"/>
-    </row>
-    <row r="22" spans="2:18" s="71" customFormat="1" ht="18.75">
-      <c r="B22" s="65"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="77" t="s">
+      <c r="F21" s="49"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
+    </row>
+    <row r="22" spans="2:18" s="67" customFormat="1" ht="18.75">
+      <c r="B22" s="61"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="68"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="69"/>
-      <c r="K22" s="69"/>
-      <c r="L22" s="70"/>
-      <c r="M22" s="70"/>
-      <c r="N22" s="70"/>
-      <c r="O22" s="70"/>
-      <c r="P22" s="70"/>
-      <c r="Q22" s="70"/>
-      <c r="R22" s="70"/>
-    </row>
-    <row r="23" spans="2:18" s="64" customFormat="1" ht="15.75">
-      <c r="B23" s="61"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72" t="s">
+      <c r="F22" s="64"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="65"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="66"/>
+    </row>
+    <row r="23" spans="2:18" s="60" customFormat="1" ht="15.75">
+      <c r="B23" s="57"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="63"/>
-      <c r="M23" s="63"/>
-      <c r="N23" s="63"/>
-      <c r="O23" s="63"/>
-      <c r="P23" s="63"/>
-      <c r="Q23" s="63"/>
-      <c r="R23" s="63"/>
-    </row>
-    <row r="24" spans="2:18" s="49" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B24" s="30"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="44"/>
-      <c r="P24" s="44"/>
-      <c r="Q24" s="44"/>
-      <c r="R24" s="44"/>
-    </row>
-    <row r="25" spans="2:18" s="49" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B25" s="30"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
-      <c r="P25" s="44"/>
-      <c r="Q25" s="44"/>
-      <c r="R25" s="44"/>
-    </row>
-    <row r="26" spans="2:18" s="49" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B26" s="30"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44"/>
-      <c r="Q26" s="44"/>
-      <c r="R26" s="44"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="59"/>
+      <c r="Q23" s="59"/>
+      <c r="R23" s="59"/>
+    </row>
+    <row r="24" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B24" s="29"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="41"/>
+      <c r="R24" s="41"/>
+    </row>
+    <row r="25" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B25" s="29"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
+    </row>
+    <row r="26" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B26" s="29"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="2" t="s">
@@ -2544,7 +2541,7 @@
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="103" t="s">
+      <c r="G27" s="82" t="s">
         <v>34</v>
       </c>
       <c r="H27" s="20"/>
@@ -2553,71 +2550,71 @@
       <c r="B28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="79" t="s">
+      <c r="C28" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="80"/>
+      <c r="D28" s="86"/>
       <c r="E28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="102" t="s">
+      <c r="F28" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="G28" s="104" t="s">
+      <c r="G28" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="104" t="s">
+      <c r="H28" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="104" t="s">
+      <c r="I28" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="104" t="s">
+      <c r="J28" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="K28" s="104" t="s">
+      <c r="K28" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="L28" s="104" t="s">
+      <c r="L28" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="M28" s="104" t="s">
+      <c r="M28" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="N28" s="104" t="s">
+      <c r="N28" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="O28" s="104" t="s">
+      <c r="O28" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="P28" s="104" t="s">
+      <c r="P28" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="Q28" s="104" t="s">
+      <c r="Q28" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="R28" s="104" t="s">
+      <c r="R28" s="83" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="12.75" customHeight="1">
       <c r="B29" s="5"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="82"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="91"/>
       <c r="E29" s="6"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="41"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39"/>
+      <c r="Q29" s="39"/>
+      <c r="R29" s="39"/>
     </row>
     <row r="30" spans="2:18" ht="14.25" customHeight="1">
       <c r="C30" s="12"/>
@@ -2651,18 +2648,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B33" s="91"/>
-      <c r="C33" s="91"/>
+    <row r="33" spans="2:18" ht="12.75" customHeight="1">
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
       <c r="D33" s="8"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="92"/>
-    </row>
-    <row r="34" spans="2:9">
+      <c r="E33" s="75"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="102"/>
+      <c r="H33" s="102"/>
+      <c r="I33" s="102"/>
+      <c r="J33" s="102"/>
+      <c r="K33" s="102"/>
+      <c r="L33" s="102"/>
+      <c r="M33" s="102"/>
+      <c r="N33" s="102"/>
+      <c r="O33" s="102"/>
+      <c r="P33" s="102"/>
+      <c r="Q33" s="102"/>
+      <c r="R33" s="102"/>
+    </row>
+    <row r="34" spans="2:18">
       <c r="B34" s="13"/>
-      <c r="G34" s="36"/>
-    </row>
-    <row r="35" spans="2:9" s="13" customFormat="1" ht="36">
+      <c r="G34" s="35"/>
+    </row>
+    <row r="35" spans="2:18" s="13" customFormat="1" ht="36">
       <c r="B35" s="16" t="s">
         <v>10</v>
       </c>
@@ -2676,581 +2685,590 @@
         <v>17</v>
       </c>
       <c r="F35"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-    </row>
-    <row r="36" spans="2:9" s="13" customFormat="1">
-      <c r="B36" s="91"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="94"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+    </row>
+    <row r="36" spans="2:18" s="13" customFormat="1">
+      <c r="B36" s="75"/>
+      <c r="C36" s="75"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="101"/>
       <c r="F36"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-    </row>
-    <row r="37" spans="2:9" s="13" customFormat="1">
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="39"/>
+      <c r="P36" s="39"/>
+      <c r="Q36" s="39"/>
+      <c r="R36" s="39"/>
+    </row>
+    <row r="37" spans="2:18" s="13" customFormat="1">
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
       <c r="F37"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-    </row>
-    <row r="38" spans="2:9" s="13" customFormat="1">
-      <c r="B38" s="35"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-    </row>
-    <row r="39" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-    </row>
-    <row r="40" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-    </row>
-    <row r="41" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-    </row>
-    <row r="42" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-    </row>
-    <row r="43" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-    </row>
-    <row r="44" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
-    </row>
-    <row r="45" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-    </row>
-    <row r="46" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
-    </row>
-    <row r="47" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
-    </row>
-    <row r="48" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+    </row>
+    <row r="38" spans="2:18" s="13" customFormat="1">
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+    </row>
+    <row r="39" spans="2:18" s="13" customFormat="1" ht="11.25">
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+    </row>
+    <row r="40" spans="2:18" s="13" customFormat="1" ht="11.25">
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+    </row>
+    <row r="41" spans="2:18" s="13" customFormat="1" ht="11.25">
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+    </row>
+    <row r="42" spans="2:18" s="13" customFormat="1" ht="11.25">
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+    </row>
+    <row r="43" spans="2:18" s="13" customFormat="1" ht="11.25">
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+    </row>
+    <row r="44" spans="2:18" s="13" customFormat="1" ht="11.25">
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+    </row>
+    <row r="45" spans="2:18" s="13" customFormat="1" ht="11.25">
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+    </row>
+    <row r="46" spans="2:18" s="13" customFormat="1" ht="11.25">
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+    </row>
+    <row r="47" spans="2:18" s="13" customFormat="1" ht="11.25">
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+    </row>
+    <row r="48" spans="2:18" s="13" customFormat="1" ht="11.25">
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
     </row>
     <row r="49" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="33"/>
-      <c r="I49" s="24"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="32"/>
+      <c r="I49" s="23"/>
     </row>
     <row r="50" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="I50" s="24"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="I50" s="23"/>
     </row>
     <row r="51" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B51" s="37"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="I51" s="24"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="I51" s="23"/>
     </row>
     <row r="52" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="I52" s="24"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="I52" s="23"/>
     </row>
     <row r="53" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
-      <c r="I53" s="24"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="I53" s="23"/>
     </row>
     <row r="54" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B54" s="37"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="I54" s="24"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="I54" s="23"/>
     </row>
     <row r="55" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="I55" s="24"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="I55" s="23"/>
     </row>
     <row r="56" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B56" s="37"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="I56" s="24"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+      <c r="I56" s="23"/>
     </row>
     <row r="57" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="38"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
-      <c r="I57" s="24"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="31"/>
+      <c r="G57" s="31"/>
+      <c r="I57" s="23"/>
     </row>
     <row r="58" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
-      <c r="I58" s="24"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="31"/>
+      <c r="I58" s="23"/>
     </row>
     <row r="59" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="32"/>
-      <c r="I59" s="24"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+      <c r="I59" s="23"/>
     </row>
     <row r="60" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
-      <c r="I60" s="24"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
+      <c r="I60" s="23"/>
     </row>
     <row r="61" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B61" s="37"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="34"/>
-      <c r="I61" s="25"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="33"/>
+      <c r="I61" s="24"/>
     </row>
     <row r="62" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="I62" s="24"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+      <c r="I62" s="23"/>
     </row>
     <row r="63" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="38"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="32"/>
-      <c r="I63" s="24"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
+      <c r="I63" s="23"/>
     </row>
     <row r="64" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="38"/>
-      <c r="E64" s="38"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="32"/>
-      <c r="I64" s="24"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+      <c r="I64" s="23"/>
     </row>
     <row r="65" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B65" s="37"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="38"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="32"/>
-      <c r="I65" s="24"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
+      <c r="I65" s="23"/>
     </row>
     <row r="66" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B66" s="37"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="33"/>
-      <c r="I66" s="24"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="31"/>
+      <c r="G66" s="32"/>
+      <c r="I66" s="23"/>
     </row>
     <row r="67" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B67" s="37"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="38"/>
-      <c r="F67" s="32"/>
-      <c r="G67" s="32"/>
-      <c r="H67" s="24"/>
-      <c r="I67" s="24"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="31"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="23"/>
+      <c r="I67" s="23"/>
     </row>
     <row r="68" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B68" s="37"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="38"/>
-      <c r="F68" s="32"/>
-      <c r="G68" s="32"/>
-      <c r="H68" s="24"/>
-      <c r="I68" s="24"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="31"/>
+      <c r="G68" s="31"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
     </row>
     <row r="69" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B69" s="37"/>
-      <c r="C69" s="37"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="38"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="33"/>
-      <c r="H69" s="24"/>
-      <c r="I69" s="24"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="31"/>
+      <c r="G69" s="32"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
     </row>
     <row r="70" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B70" s="37"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="38"/>
-      <c r="E70" s="38"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="32"/>
-      <c r="H70" s="24"/>
-      <c r="I70" s="24"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="31"/>
+      <c r="G70" s="31"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
     </row>
     <row r="71" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B71" s="37"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="38"/>
-      <c r="E71" s="38"/>
-      <c r="F71" s="34"/>
-      <c r="G71" s="32"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="24"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="36"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="31"/>
+      <c r="H71" s="23"/>
+      <c r="I71" s="23"/>
     </row>
     <row r="72" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B72" s="37"/>
-      <c r="C72" s="37"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="38"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="32"/>
-      <c r="H72" s="24"/>
-      <c r="I72" s="24"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="31"/>
+      <c r="G72" s="31"/>
+      <c r="H72" s="23"/>
+      <c r="I72" s="23"/>
     </row>
     <row r="73" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="38"/>
-      <c r="F73" s="32"/>
-      <c r="G73" s="32"/>
-      <c r="H73" s="24"/>
-      <c r="I73" s="24"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="31"/>
+      <c r="G73" s="31"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="23"/>
     </row>
     <row r="74" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B74" s="37"/>
-      <c r="C74" s="37"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="38"/>
-      <c r="F74" s="32"/>
-      <c r="G74" s="32"/>
-      <c r="H74" s="24"/>
-      <c r="I74" s="24"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="31"/>
+      <c r="G74" s="31"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="23"/>
     </row>
     <row r="75" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B75" s="37"/>
-      <c r="C75" s="37"/>
-      <c r="D75" s="38"/>
-      <c r="E75" s="38"/>
-      <c r="F75" s="32"/>
-      <c r="G75" s="33"/>
-      <c r="H75" s="24"/>
-      <c r="I75" s="24"/>
+      <c r="B75" s="36"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="31"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="23"/>
+      <c r="I75" s="23"/>
     </row>
     <row r="76" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B76" s="37"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="38"/>
-      <c r="E76" s="38"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="32"/>
-      <c r="H76" s="24"/>
-      <c r="I76" s="24"/>
+      <c r="B76" s="36"/>
+      <c r="C76" s="36"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="31"/>
+      <c r="H76" s="23"/>
+      <c r="I76" s="23"/>
     </row>
     <row r="77" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B77" s="37"/>
-      <c r="C77" s="37"/>
-      <c r="D77" s="38"/>
-      <c r="E77" s="38"/>
-      <c r="F77" s="32"/>
-      <c r="G77" s="32"/>
-      <c r="H77" s="24"/>
-      <c r="I77" s="24"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="23"/>
+      <c r="I77" s="23"/>
     </row>
     <row r="78" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="38"/>
-      <c r="E78" s="38"/>
-      <c r="F78" s="32"/>
-      <c r="G78" s="32"/>
-      <c r="H78" s="24"/>
-      <c r="I78" s="24"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="31"/>
+      <c r="G78" s="31"/>
+      <c r="H78" s="23"/>
+      <c r="I78" s="23"/>
     </row>
     <row r="79" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B79" s="37"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="38"/>
-      <c r="E79" s="38"/>
-      <c r="F79" s="32"/>
-      <c r="G79" s="32"/>
-      <c r="H79" s="24"/>
-      <c r="I79" s="24"/>
+      <c r="B79" s="36"/>
+      <c r="C79" s="36"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="31"/>
+      <c r="G79" s="31"/>
+      <c r="H79" s="23"/>
+      <c r="I79" s="23"/>
     </row>
     <row r="80" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B80" s="37"/>
-      <c r="C80" s="37"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="38"/>
-      <c r="F80" s="32"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="23"/>
-      <c r="I80" s="23"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="31"/>
+      <c r="G80" s="38"/>
+      <c r="H80" s="22"/>
+      <c r="I80" s="22"/>
     </row>
     <row r="81" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B81" s="37"/>
-      <c r="C81" s="37"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="38"/>
-      <c r="F81" s="32"/>
-      <c r="G81" s="26"/>
-      <c r="H81" s="26"/>
-      <c r="I81" s="26"/>
+      <c r="B81" s="36"/>
+      <c r="C81" s="36"/>
+      <c r="D81" s="37"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="31"/>
+      <c r="G81" s="25"/>
+      <c r="H81" s="25"/>
+      <c r="I81" s="25"/>
     </row>
     <row r="82" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B82" s="37"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="38"/>
-      <c r="F82" s="32"/>
-      <c r="G82" s="27"/>
-      <c r="H82" s="27"/>
-      <c r="I82" s="27"/>
+      <c r="B82" s="36"/>
+      <c r="C82" s="36"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="26"/>
+      <c r="H82" s="26"/>
+      <c r="I82" s="26"/>
     </row>
     <row r="83" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B83" s="37"/>
-      <c r="C83" s="37"/>
-      <c r="D83" s="38"/>
-      <c r="E83" s="38"/>
-      <c r="F83" s="32"/>
-      <c r="G83" s="27"/>
-      <c r="H83" s="27"/>
-      <c r="I83" s="27"/>
+      <c r="B83" s="36"/>
+      <c r="C83" s="36"/>
+      <c r="D83" s="37"/>
+      <c r="E83" s="37"/>
+      <c r="F83" s="31"/>
+      <c r="G83" s="26"/>
+      <c r="H83" s="26"/>
+      <c r="I83" s="26"/>
     </row>
     <row r="84" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B84" s="37"/>
-      <c r="C84" s="37"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="38"/>
-      <c r="F84" s="32"/>
-      <c r="G84" s="27"/>
-      <c r="H84" s="27"/>
-      <c r="I84" s="27"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="31"/>
+      <c r="G84" s="26"/>
+      <c r="H84" s="26"/>
+      <c r="I84" s="26"/>
     </row>
     <row r="85" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B85" s="37"/>
-      <c r="C85" s="37"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="38"/>
-      <c r="F85" s="32"/>
-      <c r="G85" s="27"/>
-      <c r="H85" s="27"/>
-      <c r="I85" s="27"/>
+      <c r="B85" s="36"/>
+      <c r="C85" s="36"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="31"/>
+      <c r="G85" s="26"/>
+      <c r="H85" s="26"/>
+      <c r="I85" s="26"/>
     </row>
     <row r="86" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B86" s="37"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="38"/>
-      <c r="F86" s="32"/>
-      <c r="G86" s="27"/>
-      <c r="H86" s="27"/>
-      <c r="I86" s="27"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="31"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="26"/>
+      <c r="I86" s="26"/>
     </row>
     <row r="87" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B87" s="37"/>
-      <c r="C87" s="37"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="38"/>
-      <c r="F87" s="32"/>
-      <c r="G87" s="28"/>
-      <c r="H87" s="28"/>
-      <c r="I87" s="28"/>
+      <c r="B87" s="36"/>
+      <c r="C87" s="36"/>
+      <c r="D87" s="37"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="31"/>
+      <c r="G87" s="27"/>
+      <c r="H87" s="27"/>
+      <c r="I87" s="27"/>
     </row>
     <row r="88" spans="2:9">
-      <c r="B88" s="37"/>
-      <c r="C88" s="37"/>
-      <c r="D88" s="38"/>
-      <c r="E88" s="38"/>
-      <c r="F88" s="32"/>
+      <c r="B88" s="36"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="31"/>
     </row>
     <row r="89" spans="2:9">
-      <c r="B89" s="37"/>
-      <c r="C89" s="37"/>
-      <c r="D89" s="38"/>
-      <c r="E89" s="38"/>
-      <c r="F89" s="32"/>
+      <c r="B89" s="36"/>
+      <c r="C89" s="36"/>
+      <c r="D89" s="37"/>
+      <c r="E89" s="37"/>
+      <c r="F89" s="31"/>
     </row>
     <row r="90" spans="2:9">
-      <c r="B90" s="37"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="39"/>
-      <c r="E90" s="39"/>
-      <c r="F90" s="39"/>
+      <c r="B90" s="36"/>
+      <c r="C90" s="36"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
     </row>
     <row r="91" spans="2:9">
-      <c r="B91" s="37"/>
-      <c r="C91" s="37"/>
-      <c r="D91" s="26"/>
-      <c r="E91" s="26"/>
-      <c r="F91" s="26"/>
+      <c r="B91" s="36"/>
+      <c r="C91" s="36"/>
+      <c r="D91" s="25"/>
+      <c r="E91" s="25"/>
+      <c r="F91" s="25"/>
     </row>
     <row r="92" spans="2:9">
-      <c r="B92" s="37"/>
-      <c r="C92" s="37"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
+      <c r="B92" s="36"/>
+      <c r="C92" s="36"/>
+      <c r="D92" s="26"/>
+      <c r="E92" s="26"/>
+      <c r="F92" s="26"/>
     </row>
     <row r="93" spans="2:9">
-      <c r="B93" s="37"/>
-      <c r="C93" s="37"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
+      <c r="B93" s="36"/>
+      <c r="C93" s="36"/>
+      <c r="D93" s="26"/>
+      <c r="E93" s="26"/>
+      <c r="F93" s="26"/>
     </row>
     <row r="94" spans="2:9">
-      <c r="B94" s="37"/>
-      <c r="C94" s="37"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="27"/>
-      <c r="F94" s="27"/>
+      <c r="B94" s="36"/>
+      <c r="C94" s="36"/>
+      <c r="D94" s="26"/>
+      <c r="E94" s="26"/>
+      <c r="F94" s="26"/>
     </row>
     <row r="95" spans="2:9">
-      <c r="B95" s="37"/>
-      <c r="C95" s="37"/>
-      <c r="D95" s="27"/>
-      <c r="E95" s="27"/>
-      <c r="F95" s="27"/>
+      <c r="B95" s="36"/>
+      <c r="C95" s="36"/>
+      <c r="D95" s="26"/>
+      <c r="E95" s="26"/>
+      <c r="F95" s="26"/>
     </row>
     <row r="96" spans="2:9">
-      <c r="B96" s="37"/>
-      <c r="C96" s="37"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27"/>
-      <c r="F96" s="27"/>
+      <c r="B96" s="36"/>
+      <c r="C96" s="36"/>
+      <c r="D96" s="26"/>
+      <c r="E96" s="26"/>
+      <c r="F96" s="26"/>
     </row>
     <row r="97" spans="2:6" customFormat="1">
-      <c r="B97" s="37"/>
-      <c r="C97" s="37"/>
-      <c r="D97" s="28"/>
-      <c r="E97" s="28"/>
-      <c r="F97" s="28"/>
+      <c r="B97" s="36"/>
+      <c r="C97" s="36"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="27"/>
+      <c r="F97" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
generate excel report 100%
</commit_message>
<xml_diff>
--- a/document/template.xlsx
+++ b/document/template.xlsx
@@ -547,7 +547,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,12 +563,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -861,14 +855,14 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="38" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="38" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="10" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -1000,16 +994,10 @@
     <xf numFmtId="186" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="186" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1031,18 +1019,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="35" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="185" fontId="35" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1100,33 +1076,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="6" fillId="8" borderId="2" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="6" fillId="7" borderId="2" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="8" borderId="11" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="6" fillId="7" borderId="11" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="8" borderId="3" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="6" fillId="7" borderId="3" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1156,14 +1123,11 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="41" fontId="51" fillId="7" borderId="2" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="51" fillId="6" borderId="2" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="51" fillId="7" borderId="3" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="51" fillId="6" borderId="3" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1181,55 +1145,26 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="48" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="34" fillId="7" borderId="11" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="34" fillId="6" borderId="11" xfId="139" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="33" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="33" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1261,17 +1196,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="33" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="8" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="35" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="185" fontId="35" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="184">
@@ -2057,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2068,7 +2053,7 @@
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="39.140625" customWidth="1"/>
-    <col min="7" max="9" width="19.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="19.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
     <col min="13" max="18" width="10.7109375" customWidth="1"/>
@@ -2076,1199 +2061,1199 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1">
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1">
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1">
-      <c r="C3" s="20"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="2:18" s="1" customFormat="1">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="74" t="s">
+      <c r="C4" s="84"/>
+      <c r="D4" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="2:18" s="1" customFormat="1">
-      <c r="B5" s="87"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:18" s="1" customFormat="1">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="2:18" s="1" customFormat="1">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="2:18" s="1" customFormat="1">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="97"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="2:18" s="1" customFormat="1">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="84" t="s">
+      <c r="C9" s="91"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="2:18">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="83" t="s">
+      <c r="C10" s="90"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="83" t="s">
+      <c r="H10" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="83" t="s">
+      <c r="I10" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="83" t="s">
+      <c r="J10" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="83" t="s">
+      <c r="K10" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="83" t="s">
+      <c r="L10" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="M10" s="83" t="s">
+      <c r="M10" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="N10" s="83" t="s">
+      <c r="N10" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="O10" s="83" t="s">
+      <c r="O10" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="P10" s="83" t="s">
+      <c r="P10" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="Q10" s="83" t="s">
+      <c r="Q10" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="R10" s="83" t="s">
+      <c r="R10" s="92" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:18" s="20" customFormat="1">
-      <c r="B11" s="30" t="s">
+    <row r="11" spans="2:18" s="14" customFormat="1">
+      <c r="B11" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="102"/>
-      <c r="M11" s="102"/>
-      <c r="N11" s="102"/>
-      <c r="O11" s="102"/>
-      <c r="P11" s="102"/>
-      <c r="Q11" s="102"/>
-      <c r="R11" s="102"/>
-    </row>
-    <row r="12" spans="2:18" s="20" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B12" s="29"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="102"/>
-      <c r="I12" s="102"/>
-      <c r="J12" s="102"/>
-      <c r="K12" s="102"/>
-      <c r="L12" s="102"/>
-      <c r="M12" s="102"/>
-      <c r="N12" s="102"/>
-      <c r="O12" s="102"/>
-      <c r="P12" s="102"/>
-      <c r="Q12" s="102"/>
-      <c r="R12" s="102"/>
-    </row>
-    <row r="13" spans="2:18" s="20" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B13" s="29"/>
-      <c r="C13" s="28"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="102"/>
-      <c r="L13" s="102"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="102"/>
-      <c r="O13" s="102"/>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="102"/>
-      <c r="R13" s="102"/>
-    </row>
-    <row r="14" spans="2:18" s="46" customFormat="1">
-      <c r="B14" s="29"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="89" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="67"/>
+    </row>
+    <row r="12" spans="2:18" s="14" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B12" s="23"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
+      <c r="R12" s="67"/>
+    </row>
+    <row r="13" spans="2:18" s="14" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B13" s="23"/>
+      <c r="C13" s="22"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="67"/>
+      <c r="R13" s="67"/>
+    </row>
+    <row r="14" spans="2:18" s="40" customFormat="1">
+      <c r="B14" s="23"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="102"/>
-      <c r="J14" s="102"/>
-      <c r="K14" s="102"/>
-      <c r="L14" s="102"/>
-      <c r="M14" s="102"/>
-      <c r="N14" s="102"/>
-      <c r="O14" s="102"/>
-      <c r="P14" s="102"/>
-      <c r="Q14" s="102"/>
-      <c r="R14" s="102"/>
-    </row>
-    <row r="15" spans="2:18" s="46" customFormat="1">
-      <c r="B15" s="29"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="89" t="s">
+      <c r="E14" s="80"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="67"/>
+      <c r="P14" s="67"/>
+      <c r="Q14" s="67"/>
+      <c r="R14" s="67"/>
+    </row>
+    <row r="15" spans="2:18" s="40" customFormat="1">
+      <c r="B15" s="23"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="41"/>
-    </row>
-    <row r="16" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B16" s="29"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="44" t="s">
+      <c r="E15" s="80"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+    </row>
+    <row r="16" spans="2:18" s="40" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B16" s="23"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
-      <c r="P16" s="41"/>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="41"/>
-    </row>
-    <row r="17" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B17" s="29"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="48" t="s">
+      <c r="F16" s="39"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+    </row>
+    <row r="17" spans="2:18" s="40" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B17" s="23"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="49"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
-    </row>
-    <row r="18" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B18" s="29"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="48" t="s">
+      <c r="F17" s="43"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+    </row>
+    <row r="18" spans="2:18" s="40" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B18" s="23"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="49"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="41"/>
-    </row>
-    <row r="19" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B19" s="29"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="48" t="s">
+      <c r="F18" s="43"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+    </row>
+    <row r="19" spans="2:18" s="40" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B19" s="23"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="49"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="41"/>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="41"/>
-    </row>
-    <row r="20" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B20" s="29"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="48" t="s">
+      <c r="F19" s="43"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
+    </row>
+    <row r="20" spans="2:18" s="40" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B20" s="23"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
-      <c r="P20" s="41"/>
-      <c r="Q20" s="41"/>
-      <c r="R20" s="41"/>
-    </row>
-    <row r="21" spans="2:18" s="46" customFormat="1">
-      <c r="B21" s="29"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="48" t="s">
+      <c r="F20" s="43"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+    </row>
+    <row r="21" spans="2:18" s="40" customFormat="1">
+      <c r="B21" s="23"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="49"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="41"/>
-    </row>
-    <row r="22" spans="2:18" s="67" customFormat="1" ht="18.75">
-      <c r="B22" s="61"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="73" t="s">
+      <c r="F21" s="43"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+    </row>
+    <row r="22" spans="2:18" s="57" customFormat="1" ht="18.75">
+      <c r="B22" s="52"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="64"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="66"/>
-      <c r="N22" s="66"/>
-      <c r="O22" s="66"/>
-      <c r="P22" s="66"/>
-      <c r="Q22" s="66"/>
-      <c r="R22" s="66"/>
-    </row>
-    <row r="23" spans="2:18" s="60" customFormat="1" ht="15.75">
-      <c r="B23" s="57"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68" t="s">
+      <c r="F22" s="55"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="56"/>
+    </row>
+    <row r="23" spans="2:18" s="51" customFormat="1" ht="15.75">
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-      <c r="J23" s="70"/>
-      <c r="K23" s="70"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59"/>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59"/>
-    </row>
-    <row r="24" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B24" s="29"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="41"/>
-    </row>
-    <row r="25" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B25" s="29"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="41"/>
-    </row>
-    <row r="26" spans="2:18" s="46" customFormat="1" ht="9.9499999999999993" customHeight="1">
-      <c r="B26" s="29"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="41"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+    </row>
+    <row r="24" spans="2:18" s="40" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B24" s="23"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+    </row>
+    <row r="25" spans="2:18" s="40" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B25" s="23"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="35"/>
+      <c r="Q25" s="35"/>
+      <c r="R25" s="35"/>
+    </row>
+    <row r="26" spans="2:18" s="40" customFormat="1" ht="9.9499999999999993" customHeight="1">
+      <c r="B26" s="23"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="82" t="s">
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="20"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="2:18" ht="12.75" customHeight="1">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="85" t="s">
+      <c r="C28" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="86"/>
-      <c r="E28" s="4" t="s">
+      <c r="D28" s="84"/>
+      <c r="E28" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="81" t="s">
+      <c r="F28" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="G28" s="83" t="s">
+      <c r="G28" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="83" t="s">
+      <c r="H28" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="83" t="s">
+      <c r="I28" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="83" t="s">
+      <c r="J28" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="K28" s="83" t="s">
+      <c r="K28" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="L28" s="83" t="s">
+      <c r="L28" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="M28" s="83" t="s">
+      <c r="M28" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="N28" s="83" t="s">
+      <c r="N28" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="O28" s="83" t="s">
+      <c r="O28" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="P28" s="83" t="s">
+      <c r="P28" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="Q28" s="83" t="s">
+      <c r="Q28" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="R28" s="83" t="s">
+      <c r="R28" s="92" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="12.75" customHeight="1">
-      <c r="B29" s="5"/>
-      <c r="C29" s="90"/>
-      <c r="D29" s="91"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="39"/>
-      <c r="R29" s="39"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="33"/>
     </row>
     <row r="30" spans="2:18" ht="14.25" customHeight="1">
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="31" spans="2:18" ht="13.5" customHeight="1">
       <c r="B31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-    </row>
-    <row r="32" spans="2:18" ht="9.9499999999999993" customHeight="1">
-      <c r="B32" s="16" t="s">
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="2:18" ht="29.25" customHeight="1">
+      <c r="B32" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="98" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="2:18" ht="12.75" customHeight="1">
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="102"/>
-      <c r="H33" s="102"/>
-      <c r="I33" s="102"/>
-      <c r="J33" s="102"/>
-      <c r="K33" s="102"/>
-      <c r="L33" s="102"/>
-      <c r="M33" s="102"/>
-      <c r="N33" s="102"/>
-      <c r="O33" s="102"/>
-      <c r="P33" s="102"/>
-      <c r="Q33" s="102"/>
-      <c r="R33" s="102"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
+      <c r="M33" s="67"/>
+      <c r="N33" s="67"/>
+      <c r="O33" s="67"/>
+      <c r="P33" s="67"/>
+      <c r="Q33" s="67"/>
+      <c r="R33" s="67"/>
     </row>
     <row r="34" spans="2:18">
-      <c r="B34" s="13"/>
-      <c r="G34" s="35"/>
-    </row>
-    <row r="35" spans="2:18" s="13" customFormat="1" ht="36">
-      <c r="B35" s="16" t="s">
+      <c r="B34" s="11"/>
+      <c r="G34" s="29"/>
+    </row>
+    <row r="35" spans="2:18" s="11" customFormat="1" ht="27.75" customHeight="1">
+      <c r="B35" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="100" t="s">
         <v>17</v>
       </c>
       <c r="F35"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-    </row>
-    <row r="36" spans="2:18" s="13" customFormat="1">
-      <c r="B36" s="75"/>
-      <c r="C36" s="75"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="101"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" spans="2:18" s="11" customFormat="1">
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="66"/>
       <c r="F36"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39"/>
-      <c r="O36" s="39"/>
-      <c r="P36" s="39"/>
-      <c r="Q36" s="39"/>
-      <c r="R36" s="39"/>
-    </row>
-    <row r="37" spans="2:18" s="13" customFormat="1">
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="33"/>
+      <c r="Q36" s="33"/>
+      <c r="R36" s="33"/>
+    </row>
+    <row r="37" spans="2:18" s="11" customFormat="1">
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
       <c r="F37"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-    </row>
-    <row r="38" spans="2:18" s="13" customFormat="1">
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-    </row>
-    <row r="39" spans="2:18" s="13" customFormat="1" ht="11.25">
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-    </row>
-    <row r="40" spans="2:18" s="13" customFormat="1" ht="11.25">
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
-    </row>
-    <row r="41" spans="2:18" s="13" customFormat="1" ht="11.25">
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-    </row>
-    <row r="42" spans="2:18" s="13" customFormat="1" ht="11.25">
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-    </row>
-    <row r="43" spans="2:18" s="13" customFormat="1" ht="11.25">
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-    </row>
-    <row r="44" spans="2:18" s="13" customFormat="1" ht="11.25">
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-    </row>
-    <row r="45" spans="2:18" s="13" customFormat="1" ht="11.25">
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-    </row>
-    <row r="46" spans="2:18" s="13" customFormat="1" ht="11.25">
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-    </row>
-    <row r="47" spans="2:18" s="13" customFormat="1" ht="11.25">
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-    </row>
-    <row r="48" spans="2:18" s="13" customFormat="1" ht="11.25">
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-    </row>
-    <row r="49" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="32"/>
-      <c r="I49" s="23"/>
-    </row>
-    <row r="50" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="I50" s="23"/>
-    </row>
-    <row r="51" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="I51" s="23"/>
-    </row>
-    <row r="52" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-      <c r="I52" s="23"/>
-    </row>
-    <row r="53" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="31"/>
-      <c r="I53" s="23"/>
-    </row>
-    <row r="54" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="I54" s="23"/>
-    </row>
-    <row r="55" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
-      <c r="I55" s="23"/>
-    </row>
-    <row r="56" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-      <c r="I56" s="23"/>
-    </row>
-    <row r="57" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="I57" s="23"/>
-    </row>
-    <row r="58" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="31"/>
-      <c r="I58" s="23"/>
-    </row>
-    <row r="59" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
-      <c r="I59" s="23"/>
-    </row>
-    <row r="60" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="37"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31"/>
-      <c r="I60" s="23"/>
-    </row>
-    <row r="61" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="31"/>
-      <c r="G61" s="33"/>
-      <c r="I61" s="24"/>
-    </row>
-    <row r="62" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31"/>
-      <c r="I62" s="23"/>
-    </row>
-    <row r="63" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="37"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31"/>
-      <c r="I63" s="23"/>
-    </row>
-    <row r="64" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="31"/>
-      <c r="G64" s="31"/>
-      <c r="I64" s="23"/>
-    </row>
-    <row r="65" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="31"/>
-      <c r="G65" s="31"/>
-      <c r="I65" s="23"/>
-    </row>
-    <row r="66" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="31"/>
-      <c r="G66" s="32"/>
-      <c r="I66" s="23"/>
-    </row>
-    <row r="67" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="31"/>
-      <c r="H67" s="23"/>
-      <c r="I67" s="23"/>
-    </row>
-    <row r="68" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
-      <c r="H68" s="23"/>
-      <c r="I68" s="23"/>
-    </row>
-    <row r="69" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="37"/>
-      <c r="F69" s="31"/>
-      <c r="G69" s="32"/>
-      <c r="H69" s="23"/>
-      <c r="I69" s="23"/>
-    </row>
-    <row r="70" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="31"/>
-      <c r="G70" s="31"/>
-      <c r="H70" s="23"/>
-      <c r="I70" s="23"/>
-    </row>
-    <row r="71" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B71" s="36"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="33"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="23"/>
-      <c r="I71" s="23"/>
-    </row>
-    <row r="72" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="37"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="31"/>
-      <c r="H72" s="23"/>
-      <c r="I72" s="23"/>
-    </row>
-    <row r="73" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B73" s="36"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31"/>
-      <c r="H73" s="23"/>
-      <c r="I73" s="23"/>
-    </row>
-    <row r="74" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31"/>
-      <c r="H74" s="23"/>
-      <c r="I74" s="23"/>
-    </row>
-    <row r="75" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="37"/>
-      <c r="E75" s="37"/>
-      <c r="F75" s="31"/>
-      <c r="G75" s="32"/>
-      <c r="H75" s="23"/>
-      <c r="I75" s="23"/>
-    </row>
-    <row r="76" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B76" s="36"/>
-      <c r="C76" s="36"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="31"/>
-      <c r="G76" s="31"/>
-      <c r="H76" s="23"/>
-      <c r="I76" s="23"/>
-    </row>
-    <row r="77" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B77" s="36"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="31"/>
-      <c r="G77" s="31"/>
-      <c r="H77" s="23"/>
-      <c r="I77" s="23"/>
-    </row>
-    <row r="78" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B78" s="36"/>
-      <c r="C78" s="36"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31"/>
-      <c r="H78" s="23"/>
-      <c r="I78" s="23"/>
-    </row>
-    <row r="79" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B79" s="36"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="37"/>
-      <c r="F79" s="31"/>
-      <c r="G79" s="31"/>
-      <c r="H79" s="23"/>
-      <c r="I79" s="23"/>
-    </row>
-    <row r="80" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B80" s="36"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="37"/>
-      <c r="F80" s="31"/>
-      <c r="G80" s="38"/>
-      <c r="H80" s="22"/>
-      <c r="I80" s="22"/>
-    </row>
-    <row r="81" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="37"/>
-      <c r="E81" s="37"/>
-      <c r="F81" s="31"/>
-      <c r="G81" s="25"/>
-      <c r="H81" s="25"/>
-      <c r="I81" s="25"/>
-    </row>
-    <row r="82" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B82" s="36"/>
-      <c r="C82" s="36"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="31"/>
-      <c r="G82" s="26"/>
-      <c r="H82" s="26"/>
-      <c r="I82" s="26"/>
-    </row>
-    <row r="83" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B83" s="36"/>
-      <c r="C83" s="36"/>
-      <c r="D83" s="37"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="31"/>
-      <c r="G83" s="26"/>
-      <c r="H83" s="26"/>
-      <c r="I83" s="26"/>
-    </row>
-    <row r="84" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="37"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="31"/>
-      <c r="G84" s="26"/>
-      <c r="H84" s="26"/>
-      <c r="I84" s="26"/>
-    </row>
-    <row r="85" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B85" s="36"/>
-      <c r="C85" s="36"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="31"/>
-      <c r="G85" s="26"/>
-      <c r="H85" s="26"/>
-      <c r="I85" s="26"/>
-    </row>
-    <row r="86" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B86" s="36"/>
-      <c r="C86" s="36"/>
-      <c r="D86" s="37"/>
-      <c r="E86" s="37"/>
-      <c r="F86" s="31"/>
-      <c r="G86" s="26"/>
-      <c r="H86" s="26"/>
-      <c r="I86" s="26"/>
-    </row>
-    <row r="87" spans="2:9" s="13" customFormat="1" ht="11.25">
-      <c r="B87" s="36"/>
-      <c r="C87" s="36"/>
-      <c r="D87" s="37"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="31"/>
-      <c r="G87" s="27"/>
-      <c r="H87" s="27"/>
-      <c r="I87" s="27"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" spans="2:18" s="11" customFormat="1">
+      <c r="B38" s="28"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+    </row>
+    <row r="39" spans="2:18" s="11" customFormat="1" ht="11.25">
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+    </row>
+    <row r="40" spans="2:18" s="11" customFormat="1" ht="11.25">
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" spans="2:18" s="11" customFormat="1" ht="11.25">
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+    </row>
+    <row r="42" spans="2:18" s="11" customFormat="1" ht="11.25">
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" spans="2:18" s="11" customFormat="1" ht="11.25">
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+    </row>
+    <row r="44" spans="2:18" s="11" customFormat="1" ht="11.25">
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+    </row>
+    <row r="45" spans="2:18" s="11" customFormat="1" ht="11.25">
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+    </row>
+    <row r="46" spans="2:18" s="11" customFormat="1" ht="11.25">
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+    </row>
+    <row r="47" spans="2:18" s="11" customFormat="1" ht="11.25">
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+    </row>
+    <row r="48" spans="2:18" s="11" customFormat="1" ht="11.25">
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+    </row>
+    <row r="49" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="26"/>
+      <c r="I49" s="17"/>
+    </row>
+    <row r="50" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="I50" s="17"/>
+    </row>
+    <row r="51" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="I51" s="17"/>
+    </row>
+    <row r="52" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="I52" s="17"/>
+    </row>
+    <row r="53" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="I53" s="17"/>
+    </row>
+    <row r="54" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="I54" s="17"/>
+    </row>
+    <row r="55" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="I55" s="17"/>
+    </row>
+    <row r="56" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
+      <c r="I56" s="17"/>
+    </row>
+    <row r="57" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B57" s="30"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25"/>
+      <c r="I57" s="17"/>
+    </row>
+    <row r="58" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="I58" s="17"/>
+    </row>
+    <row r="59" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="25"/>
+      <c r="I59" s="17"/>
+    </row>
+    <row r="60" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B60" s="30"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="25"/>
+      <c r="I60" s="17"/>
+    </row>
+    <row r="61" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B61" s="30"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="27"/>
+      <c r="I61" s="18"/>
+    </row>
+    <row r="62" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B62" s="30"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="25"/>
+      <c r="I62" s="17"/>
+    </row>
+    <row r="63" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="25"/>
+      <c r="I63" s="17"/>
+    </row>
+    <row r="64" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="31"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="25"/>
+      <c r="I64" s="17"/>
+    </row>
+    <row r="65" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B65" s="30"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="25"/>
+      <c r="I65" s="17"/>
+    </row>
+    <row r="66" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B66" s="30"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="31"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="26"/>
+      <c r="I66" s="17"/>
+    </row>
+    <row r="67" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B67" s="30"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="25"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+    </row>
+    <row r="68" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="31"/>
+      <c r="F68" s="25"/>
+      <c r="G68" s="25"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+    </row>
+    <row r="69" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B69" s="30"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+    </row>
+    <row r="70" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B70" s="30"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="31"/>
+      <c r="E70" s="31"/>
+      <c r="F70" s="25"/>
+      <c r="G70" s="25"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+    </row>
+    <row r="71" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="25"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
+    </row>
+    <row r="72" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B72" s="30"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="31"/>
+      <c r="E72" s="31"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="25"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="17"/>
+    </row>
+    <row r="73" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B73" s="30"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="31"/>
+      <c r="E73" s="31"/>
+      <c r="F73" s="25"/>
+      <c r="G73" s="25"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="17"/>
+    </row>
+    <row r="74" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B74" s="30"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="31"/>
+      <c r="E74" s="31"/>
+      <c r="F74" s="25"/>
+      <c r="G74" s="25"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+    </row>
+    <row r="75" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B75" s="30"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="25"/>
+      <c r="G75" s="26"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+    </row>
+    <row r="76" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B76" s="30"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="31"/>
+      <c r="E76" s="31"/>
+      <c r="F76" s="25"/>
+      <c r="G76" s="25"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
+    </row>
+    <row r="77" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B77" s="30"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="25"/>
+      <c r="G77" s="25"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="17"/>
+    </row>
+    <row r="78" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B78" s="30"/>
+      <c r="C78" s="30"/>
+      <c r="D78" s="31"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="25"/>
+      <c r="G78" s="25"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
+    </row>
+    <row r="79" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B79" s="30"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="31"/>
+      <c r="F79" s="25"/>
+      <c r="G79" s="25"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
+    </row>
+    <row r="80" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B80" s="30"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="31"/>
+      <c r="E80" s="31"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="32"/>
+      <c r="H80" s="16"/>
+      <c r="I80" s="16"/>
+    </row>
+    <row r="81" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B81" s="30"/>
+      <c r="C81" s="30"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="31"/>
+      <c r="F81" s="25"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="19"/>
+      <c r="I81" s="19"/>
+    </row>
+    <row r="82" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B82" s="30"/>
+      <c r="C82" s="30"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="25"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
+      <c r="I82" s="20"/>
+    </row>
+    <row r="83" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B83" s="30"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="31"/>
+      <c r="F83" s="25"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
+      <c r="I83" s="20"/>
+    </row>
+    <row r="84" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B84" s="30"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="31"/>
+      <c r="F84" s="25"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+      <c r="I84" s="20"/>
+    </row>
+    <row r="85" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="20"/>
+      <c r="H85" s="20"/>
+      <c r="I85" s="20"/>
+    </row>
+    <row r="86" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B86" s="30"/>
+      <c r="C86" s="30"/>
+      <c r="D86" s="31"/>
+      <c r="E86" s="31"/>
+      <c r="F86" s="25"/>
+      <c r="G86" s="20"/>
+      <c r="H86" s="20"/>
+      <c r="I86" s="20"/>
+    </row>
+    <row r="87" spans="2:9" s="11" customFormat="1" ht="11.25">
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="31"/>
+      <c r="F87" s="25"/>
+      <c r="G87" s="21"/>
+      <c r="H87" s="21"/>
+      <c r="I87" s="21"/>
     </row>
     <row r="88" spans="2:9">
-      <c r="B88" s="36"/>
-      <c r="C88" s="36"/>
-      <c r="D88" s="37"/>
-      <c r="E88" s="37"/>
-      <c r="F88" s="31"/>
+      <c r="B88" s="30"/>
+      <c r="C88" s="30"/>
+      <c r="D88" s="31"/>
+      <c r="E88" s="31"/>
+      <c r="F88" s="25"/>
     </row>
     <row r="89" spans="2:9">
-      <c r="B89" s="36"/>
-      <c r="C89" s="36"/>
-      <c r="D89" s="37"/>
-      <c r="E89" s="37"/>
-      <c r="F89" s="31"/>
+      <c r="B89" s="30"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="31"/>
+      <c r="F89" s="25"/>
     </row>
     <row r="90" spans="2:9">
-      <c r="B90" s="36"/>
-      <c r="C90" s="36"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="38"/>
-      <c r="F90" s="38"/>
+      <c r="B90" s="30"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="32"/>
+      <c r="E90" s="32"/>
+      <c r="F90" s="32"/>
     </row>
     <row r="91" spans="2:9">
-      <c r="B91" s="36"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
+      <c r="B91" s="30"/>
+      <c r="C91" s="30"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
     </row>
     <row r="92" spans="2:9">
-      <c r="B92" s="36"/>
-      <c r="C92" s="36"/>
-      <c r="D92" s="26"/>
-      <c r="E92" s="26"/>
-      <c r="F92" s="26"/>
+      <c r="B92" s="30"/>
+      <c r="C92" s="30"/>
+      <c r="D92" s="20"/>
+      <c r="E92" s="20"/>
+      <c r="F92" s="20"/>
     </row>
     <row r="93" spans="2:9">
-      <c r="B93" s="36"/>
-      <c r="C93" s="36"/>
-      <c r="D93" s="26"/>
-      <c r="E93" s="26"/>
-      <c r="F93" s="26"/>
+      <c r="B93" s="30"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="20"/>
     </row>
     <row r="94" spans="2:9">
-      <c r="B94" s="36"/>
-      <c r="C94" s="36"/>
-      <c r="D94" s="26"/>
-      <c r="E94" s="26"/>
-      <c r="F94" s="26"/>
+      <c r="B94" s="30"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="20"/>
+      <c r="E94" s="20"/>
+      <c r="F94" s="20"/>
     </row>
     <row r="95" spans="2:9">
-      <c r="B95" s="36"/>
-      <c r="C95" s="36"/>
-      <c r="D95" s="26"/>
-      <c r="E95" s="26"/>
-      <c r="F95" s="26"/>
+      <c r="B95" s="30"/>
+      <c r="C95" s="30"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="20"/>
     </row>
     <row r="96" spans="2:9">
-      <c r="B96" s="36"/>
-      <c r="C96" s="36"/>
-      <c r="D96" s="26"/>
-      <c r="E96" s="26"/>
-      <c r="F96" s="26"/>
+      <c r="B96" s="30"/>
+      <c r="C96" s="30"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="20"/>
     </row>
     <row r="97" spans="2:6" customFormat="1">
-      <c r="B97" s="36"/>
-      <c r="C97" s="36"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
+      <c r="B97" s="30"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="21"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>